<commit_message>
Actualización 23 de Marzo. Agrego Corea del Sur
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -182,10 +182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1293,6 +1293,65 @@
         <v>632</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>43912</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>459</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <v>746</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizado a 24 de Marzo de 2020
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -182,10 +182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="T22" activeCellId="0" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1352,6 +1352,65 @@
         <v>746</v>
       </c>
     </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>43913</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>540</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="S22" s="0" t="n">
+        <v>922</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualización 25 de Marzo
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -182,10 +182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T22" activeCellId="0" sqref="T22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26:Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1411,6 +1411,65 @@
         <v>922</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>43914</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>682</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="S23" s="0" t="n">
+        <v>1142</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Me faltó agregar el link al regional del 26
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -182,10 +182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26:Y30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K57" activeCellId="0" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1470,6 +1470,65 @@
         <v>1142</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>43915</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>746</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P24" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R24" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="S24" s="0" t="n">
+        <v>1306</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Informe al dia 28 de Marzo. Se agregan dos informes breves en formato Rnw, que sirvieron para video
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -87,7 +87,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -109,13 +109,26 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF36A9E1"/>
+        <bgColor rgb="FF00CCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,7 +165,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -165,6 +178,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -174,6 +191,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF36A9E1"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -182,10 +259,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K57" activeCellId="0" sqref="K57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="J33:Q56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1529,6 +1606,72 @@
         <v>1306</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>43916</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>938</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="P25" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R25" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="S25" s="0" t="n">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizacińo 28 de Marzo de 2020. Se agrega excel de decesos (lamentablemente, partiremos esa serie pronto)
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -87,7 +87,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -109,26 +109,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF36A9E1"/>
-        <bgColor rgb="FF00CCFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -165,7 +152,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -178,10 +165,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -191,66 +174,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF36A9E1"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -259,10 +182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="J33:Q56"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1665,12 +1588,64 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>43917</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>1084</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="S26" s="0" t="n">
+        <v>1909</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Series para el día 30 de Marzo de 2020
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -182,10 +182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N39" activeCellId="0" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1706,6 +1706,65 @@
         <v>2139</v>
       </c>
     </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>43919</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>1295</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>229</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>247</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="Q28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R28" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="S28" s="0" t="n">
+        <v>2449</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizacion a 4 de Abril. Se movieron los archivos de marzo a la carpeta marzo. Se agrega reporte diario más prueba del modelo predictivo
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -186,10 +186,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29:I30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1885,6 +1885,183 @@
       </c>
       <c r="S30" s="0" t="n">
         <v>3031</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>43922</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>1636</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>341</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>275</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>389</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <v>3404</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>43923</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>176</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>1742</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>370</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>302</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>432</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="P32" s="0" t="n">
+        <v>234</v>
+      </c>
+      <c r="Q32" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R32" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="S32" s="0" t="n">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="n">
+        <v>43924</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>1957</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>401</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>347</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <v>477</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="P33" s="0" t="n">
+        <v>259</v>
+      </c>
+      <c r="Q33" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="R33" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="S33" s="0" t="n">
+        <v>4161</v>
       </c>
     </row>
   </sheetData>
@@ -1903,10 +2080,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="I29:I30 B1"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2309,6 +2486,183 @@
         <v>16</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>43922</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>43923</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S32" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="n">
+        <v>43924</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S33" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizacion a 10 de Abril. Se incluye analisis de decesos basados en casos, muy experimental
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t xml:space="preserve">fecha</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
@@ -186,16 +183,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="40:54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="4.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="0" width="4.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="4.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
@@ -2062,6 +2061,360 @@
       </c>
       <c r="S33" s="0" t="n">
         <v>4161</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>43925</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>191</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>2102</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>425</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="N34" s="0" t="n">
+        <v>509</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="P34" s="0" t="n">
+        <v>276</v>
+      </c>
+      <c r="Q34" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R34" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="S34" s="0" t="n">
+        <v>4471</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>43926</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>2244</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>474</v>
+      </c>
+      <c r="M35" s="0" t="n">
+        <v>383</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>562</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="P35" s="0" t="n">
+        <v>286</v>
+      </c>
+      <c r="Q35" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R35" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="S35" s="0" t="n">
+        <v>4815</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>43927</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>214</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>2350</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>522</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <v>410</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>612</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="P36" s="0" t="n">
+        <v>299</v>
+      </c>
+      <c r="Q36" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R36" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="S36" s="0" t="n">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="n">
+        <v>43928</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>225</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>2548</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>561</v>
+      </c>
+      <c r="M37" s="0" t="n">
+        <v>439</v>
+      </c>
+      <c r="N37" s="0" t="n">
+        <v>669</v>
+      </c>
+      <c r="O37" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="P37" s="0" t="n">
+        <v>325</v>
+      </c>
+      <c r="Q37" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R37" s="0" t="n">
+        <v>266</v>
+      </c>
+      <c r="S37" s="0" t="n">
+        <v>5546</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
+        <v>43929</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>2832</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>571</v>
+      </c>
+      <c r="M38" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>689</v>
+      </c>
+      <c r="O38" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="P38" s="0" t="n">
+        <v>340</v>
+      </c>
+      <c r="Q38" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R38" s="0" t="n">
+        <v>286</v>
+      </c>
+      <c r="S38" s="0" t="n">
+        <v>5972</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <v>43930</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>3193</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>589</v>
+      </c>
+      <c r="M39" s="0" t="n">
+        <v>474</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <v>712</v>
+      </c>
+      <c r="O39" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="P39" s="0" t="n">
+        <v>349</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R39" s="0" t="n">
+        <v>331</v>
+      </c>
+      <c r="S39" s="0" t="n">
+        <v>6501</v>
       </c>
     </row>
   </sheetData>
@@ -2080,10 +2433,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="40:54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2149,7 +2502,7 @@
         <v>17</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2159,6 +2512,57 @@
       <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -2167,6 +2571,57 @@
       <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -2175,6 +2630,57 @@
       <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -2183,6 +2689,57 @@
       <c r="B5" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -2191,6 +2748,57 @@
       <c r="B6" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -2199,6 +2807,57 @@
       <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -2207,6 +2866,57 @@
       <c r="B8" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -2215,6 +2925,57 @@
       <c r="B9" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -2223,6 +2984,57 @@
       <c r="B10" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -2231,6 +3043,57 @@
       <c r="B11" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -2239,6 +3102,57 @@
       <c r="B12" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -2247,6 +3161,57 @@
       <c r="B13" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -2255,6 +3220,57 @@
       <c r="B14" s="1" t="n">
         <v>13</v>
       </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -2263,6 +3279,57 @@
       <c r="B15" s="1" t="n">
         <v>14</v>
       </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -2271,6 +3338,57 @@
       <c r="B16" s="1" t="n">
         <v>15</v>
       </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -2279,6 +3397,57 @@
       <c r="B17" s="1" t="n">
         <v>16</v>
       </c>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -2287,6 +3456,57 @@
       <c r="B18" s="1" t="n">
         <v>17</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -2295,6 +3515,57 @@
       <c r="B19" s="1" t="n">
         <v>18</v>
       </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -2303,6 +3574,57 @@
       <c r="B20" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -2311,6 +3633,57 @@
       <c r="B21" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -2319,6 +3692,57 @@
       <c r="B22" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="C22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -2327,6 +3751,57 @@
       <c r="B23" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="C23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -2335,6 +3810,57 @@
       <c r="B24" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="C24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -2343,6 +3869,57 @@
       <c r="B25" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
@@ -2351,6 +3928,57 @@
       <c r="B26" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
@@ -2359,6 +3987,57 @@
       <c r="B27" s="0" t="n">
         <v>26</v>
       </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
@@ -2367,6 +4046,57 @@
       <c r="B28" s="0" t="n">
         <v>27</v>
       </c>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
@@ -2661,6 +4391,360 @@
       </c>
       <c r="S33" s="0" t="n">
         <v>27</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>43925</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N34" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S34" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>43926</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="M35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S35" s="0" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>43927</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S36" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="n">
+        <v>43928</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="M37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N37" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="O37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S37" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
+        <v>43929</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="O38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S38" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <v>43930</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="O39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S39" s="0" t="n">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion a 14 de Abril. Agregué gráfico de aceleración vs cuadrático
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -183,10 +183,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="40:54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG52" activeCellId="0" sqref="A52:AG54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2415,6 +2415,242 @@
       </c>
       <c r="S39" s="0" t="n">
         <v>6501</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
+        <v>43931</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>248</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>3448</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>606</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <v>490</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>739</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="P40" s="0" t="n">
+        <v>364</v>
+      </c>
+      <c r="Q40" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R40" s="0" t="n">
+        <v>377</v>
+      </c>
+      <c r="S40" s="0" t="n">
+        <v>6927</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="n">
+        <v>43932</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>254</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>3599</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>613</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>775</v>
+      </c>
+      <c r="O41" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="P41" s="0" t="n">
+        <v>372</v>
+      </c>
+      <c r="Q41" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R41" s="0" t="n">
+        <v>396</v>
+      </c>
+      <c r="S41" s="0" t="n">
+        <v>7213</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="n">
+        <v>43933</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>273</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>3803</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>618</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="N42" s="0" t="n">
+        <v>795</v>
+      </c>
+      <c r="O42" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="P42" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="Q42" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R42" s="0" t="n">
+        <v>415</v>
+      </c>
+      <c r="S42" s="0" t="n">
+        <v>7525</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="n">
+        <v>43934</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>155</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>285</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>4086</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>622</v>
+      </c>
+      <c r="M43" s="0" t="n">
+        <v>528</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <v>816</v>
+      </c>
+      <c r="O43" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="P43" s="0" t="n">
+        <v>385</v>
+      </c>
+      <c r="Q43" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R43" s="0" t="n">
+        <v>429</v>
+      </c>
+      <c r="S43" s="0" t="n">
+        <v>7917</v>
       </c>
     </row>
   </sheetData>
@@ -2433,10 +2669,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="40:54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="1" sqref="A52:AG54 A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4747,6 +4983,242 @@
         <v>65</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
+        <v>43931</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P40" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S40" s="0" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="n">
+        <v>43932</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="O41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P41" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S41" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="n">
+        <v>43933</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N42" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="O42" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P42" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="S42" s="0" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="n">
+        <v>43934</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="M43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="O43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P43" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S43" s="0" t="n">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizacion 15 de Abril. Agregue animación de la formula cuadratica. Requiere mayor desarrollo, pero no se ve mal....
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -183,10 +183,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG52" activeCellId="0" sqref="A52:AG54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC57" activeCellId="0" sqref="A51:AC57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2651,6 +2651,65 @@
       </c>
       <c r="S43" s="0" t="n">
         <v>7917</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
+        <v>43935</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>176</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>299</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>4334</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <v>634</v>
+      </c>
+      <c r="M44" s="0" t="n">
+        <v>542</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>826</v>
+      </c>
+      <c r="O44" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="P44" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="Q44" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R44" s="0" t="n">
+        <v>444</v>
+      </c>
+      <c r="S44" s="0" t="n">
+        <v>8273</v>
       </c>
     </row>
   </sheetData>
@@ -2669,10 +2728,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="1" sqref="A52:AG54 A41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="1" sqref="A51:AC57 A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5219,6 +5278,65 @@
         <v>92</v>
       </c>
     </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
+        <v>43935</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="M44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="O44" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P44" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S44" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizacion 16 de Abril de 2020. Nueva prueba de modelo predictivo. Informe nuevo, que agrega modelo cuadrático
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -183,10 +183,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC57" activeCellId="0" sqref="A51:AC57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="46:60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2710,6 +2710,65 @@
       </c>
       <c r="S44" s="0" t="n">
         <v>8273</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="n">
+        <v>43936</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>330</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>4682</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="L45" s="0" t="n">
+        <v>639</v>
+      </c>
+      <c r="M45" s="0" t="n">
+        <v>559</v>
+      </c>
+      <c r="N45" s="0" t="n">
+        <v>882</v>
+      </c>
+      <c r="O45" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="P45" s="0" t="n">
+        <v>399</v>
+      </c>
+      <c r="Q45" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R45" s="0" t="n">
+        <v>467</v>
+      </c>
+      <c r="S45" s="0" t="n">
+        <v>8807</v>
       </c>
     </row>
   </sheetData>
@@ -2728,10 +2787,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="1" sqref="A51:AC57 A42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N45" activeCellId="1" sqref="46:60 N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5337,6 +5396,65 @@
         <v>94</v>
       </c>
     </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="n">
+        <v>43936</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L45" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="M45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N45" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="O45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P45" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S45" s="0" t="n">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualización 18 de Octubre
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -183,10 +183,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S45"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="46:60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2769,6 +2769,124 @@
       </c>
       <c r="S45" s="0" t="n">
         <v>8807</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="n">
+        <v>43937</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>345</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>4915</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <v>223</v>
+      </c>
+      <c r="L46" s="0" t="n">
+        <v>656</v>
+      </c>
+      <c r="M46" s="0" t="n">
+        <v>578</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <v>907</v>
+      </c>
+      <c r="O46" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="P46" s="0" t="n">
+        <v>412</v>
+      </c>
+      <c r="Q46" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R46" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="S46" s="0" t="n">
+        <v>9252</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="n">
+        <v>43938</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>226</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>359</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>5192</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <v>276</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <v>667</v>
+      </c>
+      <c r="M47" s="0" t="n">
+        <v>606</v>
+      </c>
+      <c r="N47" s="0" t="n">
+        <v>944</v>
+      </c>
+      <c r="O47" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="P47" s="0" t="n">
+        <v>416</v>
+      </c>
+      <c r="Q47" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R47" s="0" t="n">
+        <v>522</v>
+      </c>
+      <c r="S47" s="0" t="n">
+        <v>9730</v>
       </c>
     </row>
   </sheetData>
@@ -2787,10 +2905,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S45"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N45" activeCellId="1" sqref="46:60 N45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5455,6 +5573,124 @@
         <v>105</v>
       </c>
     </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="n">
+        <v>43937</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L46" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="O46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P46" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S46" s="0" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="n">
+        <v>43938</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M47" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N47" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="O47" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P47" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R47" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S47" s="0" t="n">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizacion a 22 de Abril de 2020
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -183,10 +183,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA62" activeCellId="0" sqref="A56:AA62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2887,6 +2887,242 @@
       </c>
       <c r="S47" s="0" t="n">
         <v>9730</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="n">
+        <v>43939</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>249</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>381</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>5381</v>
+      </c>
+      <c r="J48" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <v>302</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <v>678</v>
+      </c>
+      <c r="M48" s="0" t="n">
+        <v>616</v>
+      </c>
+      <c r="N48" s="0" t="n">
+        <v>972</v>
+      </c>
+      <c r="O48" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="P48" s="0" t="n">
+        <v>421</v>
+      </c>
+      <c r="Q48" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R48" s="0" t="n">
+        <v>553</v>
+      </c>
+      <c r="S48" s="0" t="n">
+        <v>10088</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="n">
+        <v>43940</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>388</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>5643</v>
+      </c>
+      <c r="J49" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="K49" s="0" t="n">
+        <v>304</v>
+      </c>
+      <c r="L49" s="0" t="n">
+        <v>687</v>
+      </c>
+      <c r="M49" s="0" t="n">
+        <v>626</v>
+      </c>
+      <c r="N49" s="0" t="n">
+        <v>1045</v>
+      </c>
+      <c r="O49" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="P49" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="Q49" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R49" s="0" t="n">
+        <v>566</v>
+      </c>
+      <c r="S49" s="0" t="n">
+        <v>10507</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="n">
+        <v>43941</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>291</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>403</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>5788</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <v>694</v>
+      </c>
+      <c r="M50" s="0" t="n">
+        <v>636</v>
+      </c>
+      <c r="N50" s="0" t="n">
+        <v>1092</v>
+      </c>
+      <c r="O50" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="P50" s="0" t="n">
+        <v>432</v>
+      </c>
+      <c r="Q50" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R50" s="0" t="n">
+        <v>593</v>
+      </c>
+      <c r="S50" s="0" t="n">
+        <v>10832</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="n">
+        <v>43942</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>326</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>421</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>6083</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <v>328</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <v>703</v>
+      </c>
+      <c r="M51" s="0" t="n">
+        <v>658</v>
+      </c>
+      <c r="N51" s="0" t="n">
+        <v>1113</v>
+      </c>
+      <c r="O51" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="P51" s="0" t="n">
+        <v>445</v>
+      </c>
+      <c r="Q51" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R51" s="0" t="n">
+        <v>605</v>
+      </c>
+      <c r="S51" s="0" t="n">
+        <v>11296</v>
       </c>
     </row>
   </sheetData>
@@ -2905,10 +3141,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T49" activeCellId="1" sqref="A56:AA62 T49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5691,6 +5927,242 @@
         <v>126</v>
       </c>
     </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="n">
+        <v>43939</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="J48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N48" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="O48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P48" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R48" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S48" s="0" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="n">
+        <v>43940</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="J49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L49" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N49" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="O49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P49" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R49" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="S49" s="0" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="n">
+        <v>43941</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M50" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N50" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="O50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P50" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R50" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S50" s="0" t="n">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="n">
+        <v>43942</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M51" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N51" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="O51" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P51" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R51" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S51" s="0" t="n">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualización 28 de abril de 2020
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -183,10 +183,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA62" activeCellId="0" sqref="A56:AA62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA66" activeCellId="1" sqref="A55:B57 AA66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -197,7 +197,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="4.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,6 +3125,360 @@
       </c>
       <c r="S51" s="0" t="n">
         <v>11296</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="n">
+        <v>43943</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>340</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>429</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>6434</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <v>333</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <v>708</v>
+      </c>
+      <c r="M52" s="0" t="n">
+        <v>675</v>
+      </c>
+      <c r="N52" s="0" t="n">
+        <v>1142</v>
+      </c>
+      <c r="O52" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="P52" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="Q52" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R52" s="0" t="n">
+        <v>615</v>
+      </c>
+      <c r="S52" s="0" t="n">
+        <v>11812</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="n">
+        <v>43944</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>436</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>6761</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>349</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <v>715</v>
+      </c>
+      <c r="M53" s="0" t="n">
+        <v>683</v>
+      </c>
+      <c r="N53" s="0" t="n">
+        <v>1184</v>
+      </c>
+      <c r="O53" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="P53" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="Q53" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R53" s="0" t="n">
+        <v>624</v>
+      </c>
+      <c r="S53" s="0" t="n">
+        <v>12306</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="n">
+        <v>43945</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>391</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>7165</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <v>725</v>
+      </c>
+      <c r="M54" s="0" t="n">
+        <v>696</v>
+      </c>
+      <c r="N54" s="0" t="n">
+        <v>1203</v>
+      </c>
+      <c r="O54" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="P54" s="0" t="n">
+        <v>465</v>
+      </c>
+      <c r="Q54" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R54" s="0" t="n">
+        <v>655</v>
+      </c>
+      <c r="S54" s="0" t="n">
+        <v>12858</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="n">
+        <v>43946</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>252</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>443</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>7496</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <v>354</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <v>731</v>
+      </c>
+      <c r="M55" s="0" t="n">
+        <v>703</v>
+      </c>
+      <c r="N55" s="0" t="n">
+        <v>1216</v>
+      </c>
+      <c r="O55" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="P55" s="0" t="n">
+        <v>473</v>
+      </c>
+      <c r="Q55" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R55" s="0" t="n">
+        <v>668</v>
+      </c>
+      <c r="S55" s="0" t="n">
+        <v>13331</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="n">
+        <v>43947</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>457</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>485</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>7858</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <v>363</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <v>741</v>
+      </c>
+      <c r="M56" s="0" t="n">
+        <v>706</v>
+      </c>
+      <c r="N56" s="0" t="n">
+        <v>1236</v>
+      </c>
+      <c r="O56" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="P56" s="0" t="n">
+        <v>477</v>
+      </c>
+      <c r="Q56" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R56" s="0" t="n">
+        <v>671</v>
+      </c>
+      <c r="S56" s="0" t="n">
+        <v>13813</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="n">
+        <v>43948</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>268</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>169</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>481</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>493</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>8300</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>384</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <v>747</v>
+      </c>
+      <c r="M57" s="0" t="n">
+        <v>709</v>
+      </c>
+      <c r="N57" s="0" t="n">
+        <v>1251</v>
+      </c>
+      <c r="O57" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="P57" s="0" t="n">
+        <v>477</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R57" s="0" t="n">
+        <v>693</v>
+      </c>
+      <c r="S57" s="0" t="n">
+        <v>14365</v>
       </c>
     </row>
   </sheetData>
@@ -3141,10 +3497,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T49" activeCellId="1" sqref="A56:AA62 T49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6163,6 +6519,360 @@
         <v>160</v>
       </c>
     </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="n">
+        <v>43943</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M52" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N52" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="O52" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P52" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R52" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S52" s="0" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="n">
+        <v>43944</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M53" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N53" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="O53" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P53" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R53" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="S53" s="0" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="n">
+        <v>43945</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M54" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N54" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="O54" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P54" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R54" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="S54" s="0" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="n">
+        <v>43946</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M55" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N55" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="O55" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P55" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R55" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="S55" s="0" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="n">
+        <v>43947</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M56" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N56" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="O56" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P56" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R56" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="S56" s="0" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="n">
+        <v>43948</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M57" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N57" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="O57" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P57" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R57" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="S57" s="0" t="n">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizacion 7 de Mayo 2020
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="casos_totales" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="decesos" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="casos_asintomaticos" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,8 +21,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="I58" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Se agregan 250 casos asintomáticos
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S59" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Considera casos asintomáticos en el total
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t xml:space="preserve">fecha</t>
   </si>
@@ -111,12 +150,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,7 +198,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -166,6 +211,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -175,6 +224,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -183,16 +292,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA66" activeCellId="1" sqref="A55:B57 AA66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M67" activeCellId="0" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="0" width="4.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="4.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="8.66"/>
@@ -3481,6 +3592,537 @@
         <v>14365</v>
       </c>
     </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="n">
+        <v>43949</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>272</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>514</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>526</v>
+      </c>
+      <c r="I58" s="3" t="n">
+        <v>8889</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>392</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>761</v>
+      </c>
+      <c r="M58" s="0" t="n">
+        <v>719</v>
+      </c>
+      <c r="N58" s="0" t="n">
+        <v>1273</v>
+      </c>
+      <c r="O58" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="P58" s="0" t="n">
+        <v>481</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R58" s="0" t="n">
+        <v>714</v>
+      </c>
+      <c r="S58" s="0" t="n">
+        <v>15135</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="n">
+        <v>43950</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>279</v>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>198</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>546</v>
+      </c>
+      <c r="F59" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="G59" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>559</v>
+      </c>
+      <c r="I59" s="3" t="n">
+        <v>9625</v>
+      </c>
+      <c r="J59" s="3" t="n">
+        <v>108</v>
+      </c>
+      <c r="K59" s="3" t="n">
+        <v>393</v>
+      </c>
+      <c r="L59" s="3" t="n">
+        <v>768</v>
+      </c>
+      <c r="M59" s="3" t="n">
+        <v>727</v>
+      </c>
+      <c r="N59" s="3" t="n">
+        <v>1293</v>
+      </c>
+      <c r="O59" s="3" t="n">
+        <v>189</v>
+      </c>
+      <c r="P59" s="3" t="n">
+        <v>487</v>
+      </c>
+      <c r="Q59" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="R59" s="3" t="n">
+        <v>725</v>
+      </c>
+      <c r="S59" s="3" t="n">
+        <v>16023</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="n">
+        <v>43951</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>297</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>589</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>568</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>10516</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>394</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <v>768</v>
+      </c>
+      <c r="M60" s="0" t="n">
+        <v>729</v>
+      </c>
+      <c r="N60" s="0" t="n">
+        <v>1295</v>
+      </c>
+      <c r="O60" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="P60" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="Q60" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R60" s="0" t="n">
+        <v>726</v>
+      </c>
+      <c r="S60" s="0" t="n">
+        <v>17008</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="n">
+        <v>43952</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>307</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>212</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>679</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <v>614</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>11661</v>
+      </c>
+      <c r="J61" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <v>396</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <v>776</v>
+      </c>
+      <c r="M61" s="0" t="n">
+        <v>751</v>
+      </c>
+      <c r="N61" s="0" t="n">
+        <v>1314</v>
+      </c>
+      <c r="O61" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="P61" s="0" t="n">
+        <v>513</v>
+      </c>
+      <c r="Q61" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R61" s="0" t="n">
+        <v>752</v>
+      </c>
+      <c r="S61" s="0" t="n">
+        <v>18435</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="n">
+        <v>43953</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>272</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>740</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>638</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>12656</v>
+      </c>
+      <c r="J62" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="K62" s="0" t="n">
+        <v>397</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <v>786</v>
+      </c>
+      <c r="M62" s="0" t="n">
+        <v>759</v>
+      </c>
+      <c r="N62" s="0" t="n">
+        <v>1328</v>
+      </c>
+      <c r="O62" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="P62" s="0" t="n">
+        <v>517</v>
+      </c>
+      <c r="Q62" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R62" s="0" t="n">
+        <v>777</v>
+      </c>
+      <c r="S62" s="0" t="n">
+        <v>19663</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="n">
+        <v>43954</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>295</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>760</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>656</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>13528</v>
+      </c>
+      <c r="J63" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="K63" s="0" t="n">
+        <v>399</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <v>787</v>
+      </c>
+      <c r="M63" s="0" t="n">
+        <v>762</v>
+      </c>
+      <c r="N63" s="0" t="n">
+        <v>1331</v>
+      </c>
+      <c r="O63" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="P63" s="0" t="n">
+        <v>524</v>
+      </c>
+      <c r="Q63" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R63" s="0" t="n">
+        <v>795</v>
+      </c>
+      <c r="S63" s="0" t="n">
+        <v>20643</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="n">
+        <v>43955</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>322</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>811</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>687</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>14707</v>
+      </c>
+      <c r="J64" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="K64" s="0" t="n">
+        <v>408</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <v>789</v>
+      </c>
+      <c r="M64" s="0" t="n">
+        <v>774</v>
+      </c>
+      <c r="N64" s="0" t="n">
+        <v>1352</v>
+      </c>
+      <c r="O64" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="P64" s="0" t="n">
+        <v>525</v>
+      </c>
+      <c r="Q64" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R64" s="0" t="n">
+        <v>809</v>
+      </c>
+      <c r="S64" s="0" t="n">
+        <v>22016</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="n">
+        <v>43956</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>339</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>855</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <v>716</v>
+      </c>
+      <c r="I65" s="0" t="n">
+        <v>15582</v>
+      </c>
+      <c r="J65" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="K65" s="0" t="n">
+        <v>408</v>
+      </c>
+      <c r="L65" s="0" t="n">
+        <v>791</v>
+      </c>
+      <c r="M65" s="0" t="n">
+        <v>789</v>
+      </c>
+      <c r="N65" s="0" t="n">
+        <v>1362</v>
+      </c>
+      <c r="O65" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P65" s="0" t="n">
+        <v>541</v>
+      </c>
+      <c r="Q65" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R65" s="0" t="n">
+        <v>818</v>
+      </c>
+      <c r="S65" s="0" t="n">
+        <v>23048</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="n">
+        <v>43957</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>325</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>417</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>895</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <v>781</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <v>16828</v>
+      </c>
+      <c r="J66" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="K66" s="0" t="n">
+        <v>414</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <v>793</v>
+      </c>
+      <c r="M66" s="0" t="n">
+        <v>814</v>
+      </c>
+      <c r="N66" s="0" t="n">
+        <v>1385</v>
+      </c>
+      <c r="O66" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="P66" s="0" t="n">
+        <v>545</v>
+      </c>
+      <c r="Q66" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R66" s="0" t="n">
+        <v>836</v>
+      </c>
+      <c r="S66" s="0" t="n">
+        <v>24581</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3489,6 +4131,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3497,10 +4140,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55:B57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6873,6 +7516,1622 @@
         <v>207</v>
       </c>
     </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="n">
+        <v>43949</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M58" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N58" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="O58" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P58" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S58" s="0" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="n">
+        <v>43950</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M59" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N59" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="O59" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P59" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R59" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S59" s="0" t="n">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="n">
+        <v>43951</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M60" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N60" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="O60" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P60" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R60" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S60" s="0" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="n">
+        <v>43952</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="J61" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M61" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N61" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="O61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P61" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R61" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S61" s="0" t="n">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="n">
+        <v>43953</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="J62" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K62" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M62" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N62" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="O62" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P62" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R62" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S62" s="0" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="n">
+        <v>43954</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="J63" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K63" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M63" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N63" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="O63" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P63" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R63" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S63" s="0" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="n">
+        <v>43955</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="J64" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K64" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M64" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N64" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="O64" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P64" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R64" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S64" s="0" t="n">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="n">
+        <v>43956</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="I65" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="J65" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K65" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L65" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M65" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N65" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="O65" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P65" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R65" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S65" s="0" t="n">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="n">
+        <v>43957</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="J66" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K66" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M66" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N66" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="O66" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P66" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R66" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S66" s="0" t="n">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S66"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="3" style="0" width="6.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>43893</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>43894</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>43895</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>43896</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>43897</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>43898</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>43899</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>43900</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>43901</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>43902</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>43903</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>43904</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>43905</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>43906</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>43907</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>43908</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>43909</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>43910</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>43911</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>43912</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>43913</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>43914</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>43915</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>43916</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>43917</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>43918</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>43919</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>43920</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>43921</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>43922</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>43923</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="n">
+        <v>43924</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>43925</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>43926</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>43927</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="n">
+        <v>43928</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
+        <v>43929</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <v>43930</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
+        <v>43931</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="n">
+        <v>43932</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="n">
+        <v>43933</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="n">
+        <v>43934</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
+        <v>43935</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="n">
+        <v>43936</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="n">
+        <v>43937</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="n">
+        <v>43938</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="n">
+        <v>43939</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="n">
+        <v>43940</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="n">
+        <v>43941</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="n">
+        <v>43942</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="n">
+        <v>43943</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="n">
+        <v>43944</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="n">
+        <v>43945</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="n">
+        <v>43946</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="n">
+        <v>43947</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="n">
+        <v>43948</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="n">
+        <v>43949</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="n">
+        <v>43950</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N59" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" s="0" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="n">
+        <v>43951</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" s="0" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="n">
+        <v>43952</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="J61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="M61" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S61" s="0" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="n">
+        <v>43953</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="J62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" s="0" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="n">
+        <v>43954</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="J63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N63" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P63" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S63" s="0" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="n">
+        <v>43955</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="J64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N64" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S64" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="n">
+        <v>43956</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I65" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="J65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M65" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N65" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P65" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S65" s="0" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="n">
+        <v>43957</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="J66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M66" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N66" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="O66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R66" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S66" s="0" t="n">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizado 15 de Mayo 2020
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -11,6 +11,7 @@
     <sheet name="casos_totales" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="decesos" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="casos_asintomaticos" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="discurso" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
   <si>
     <t xml:space="preserve">fecha</t>
   </si>
@@ -118,6 +119,153 @@
   <si>
     <t xml:space="preserve">total</t>
   </si>
+  <si>
+    <t xml:space="preserve">Fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explicacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fase 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gobierno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.minsal.cl/coronavirus-en-chile-pasa-a-fase-4-y-presidente-anuncia-cierre-de-fronteras/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué pasa si el virus se vuelve buena persona?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mañalich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.24horas.cl/coronavirus/manalich-y-solicitudes-de-cuarentena-total-es-completamente-insensato-e-innecesario-4037205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se entregará Carnet COVID-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Estas personas con este carnet de alta van a quedar liberadas de todo tipo de cuarentena o restricción, porque precisamente ellas pueden ayudar enormemente a la comunidad, porque no presentan un riesgo”, explicó el secretario de Estado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.minsal.cl/ministerio-de-salud-entregara-carnet-sanitario-a-los-recuperados-de-covid-19/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nueva Normalidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“no vamos a poder volver a nuestras vidas normales como eran antes, vamos a tener que acostumbrarnos a una nueva normalidad”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piñera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ellibero.cl/alerta/presidente-pinera-tendremos-que-acostumbrarnos-a-una-nueva-normalidad/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Café de Daza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“¿Me puedo juntar con un grupo de amigo a tomar un café? probablemente si, con unos pocos amigos, con cuatro amigos, con un distanciamiento social que tengamos dos metros de distancia para poder conversar. Con mascarillas, con lavado de mano, manteniendo esas medidas”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.elmostrador.cl/noticias/multimedia/2020/04/20/paula-daza-dice-que-es-posible-salir-a-tomar-un-cafe-con-amigos-manteniendo-los-resguardos-necesarios-para-evitar-contagios/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerveza de Mañalich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"La subsecretaria Daza tiene una debilidad enorme por el café y, en ese sentido, yo la comprendo. Puede haber múltiples ejemplos, puede ser ir a tomar cerveza, por ejemplo, ir a comerse una empanada". señaló el secretario de Estado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.meganoticias.cl/nacional/299323-nueva-normalidad-cerveza-empanada-manalich-daza-cafe-coronavirus.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retorno Seguro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Mandatario detalló que el plan prioriza la salud de todos los chilenos, será gradual y flexible. El programa busca impulsar un regreso gradual a sus labores de los funcionarios públicos, trabajadores del sector privado y sociedad civil, y de los estudiantes a los recintos educacionales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://prensa.presidencia.cl/comunicado.aspx?id=150453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No es el momento, de Torrealba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Tal vez hoy no es el momento para exigir ese tipo de información con ese alto nivel de exigencia de entrega", dijo este viernes la subsecretaria de Ciencia, Tecnología, Conocimiento e Innovación, Carolina Torrealba, consultada por el congelamiento de la participación del Instituto Milenio Fundamentos de los Datos (IMFD) en la Mesa de Datos Covid-19.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torrealba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.latercera.com/politica/noticia/subsecretaria-de-ciencias-defiende-al-gobierno-tras-quiebre-de-mesa-de-datos-covid-19-tal-vez-hoy-no-es-el-momento-para-exigir-ese-tipo-de-informacion/OS2TDSCK3JEKPHWZTBBFW3Y7TU/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batalla de Santiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Esto es una receta para el fracaso: si no damos en serio con toda la energía la 'batalla de Santiago', la guerra del COVID se va a perder”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.24horas.cl/coronavirus/jaime-manalich-si-no-damos-con-toda-la-energia-la-batalla-de-santiago-la-guerra-del-covid-19-se-va-a-perder-4143993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irresponsabilidad de los habitantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“El Presidente Piñera dio a conocer seis nuevas comunas o parte de ellas, que se someterán a cuarentena a partir del martes a las 22.00 que se sumarán a las 14 comunas ya vigentes con cuarentena en el país. Esto producto de la irresponsabilidad con que, principalmente los habitantes de la Región Metropolitana, enfrentan las medidas restrictivas y de autocuidado instruidas por la autoridad sanitaria”. Esta explicación se lee en uno de los párrafos de la minuta de contingencia diaria que elabora el gobierno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.latercera.com/la-tercera-pm/noticia/irresponsabilidad-de-la-ciudadania-y-aumento-de-casos-por-que-la-moneda-se-alejo-del-retorno-seguro/IZRRR2OPKZFMHMISO2TIUCTKVU/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Pepsi o Coca-Cola?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consultado por el tema, el secretario de Estado ironizó: "lo que coma cada persona que no está en cuarentena, la bebida que tome en realidad no es nuestra preocupación. De hecho los decretos que emanamos cada día no hacen un listado de lo que se puede o no se puede consumir en estos locales. Si a alguien le gusta más la Coca Cola o la Pepsi Cola, nosotros no lo vamos a poner en un decreto”.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.meganoticias.cl/nacional/300728-jaime-manalich-ejemplos-de-nueva-normalidad-cafe-empanadas.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se suspende Carnet COVID-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El secretario de estado aseguró que decisión se fundamenta en que “se nos ha hecho ver que podría desencadenarse un problema de discriminación bastante severo”.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.latercera.com/nacional/noticia/gobierno-da-marcha-atras-y-anuncia-que-no-se-implementara-el-carnet-covid-en-chile-se-nos-ha-hecho-ver-que-podria-desencadenarse-un-problema-de-discriminatorio-bastante-severo/VQHWCSE2ZVGJPNBEBSML2FHZ5A/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuarenta total para RM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.biobiochile.cl/noticias/nacional/chile/2020/05/13/decretan-cuarentena-para-gran-santiago-y-otras-6-comunas-de-la-rm-se-suma-iquique-y-alto-hospicio.shtml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La falta de confianza recíproca nos jugó una mala pasada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Decirle a la gente que confíe en lo que el Estado le dice como conducta correcta es muy difícil. Ese trasfondo de falta de confianza recíproca nos jugó una mala pasada en la lucha contra esta pandemia", sostuvo Mañalich. La autoridad agregó que "creo que no hemos logrado encontrar un mecanismo de diálogo con la ciudadanía, transparente y de buena fe".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.elmostrador.cl/noticias/pais/2020/05/14/manalich-intensamente-preocupado-ministro-apunta-a-falta-de-confianza-reciproca-para-explicar-el-complejo-cuadro-en-la-lucha-contra-el-covid-19/</t>
+  </si>
 </sst>
 </file>
 
@@ -127,7 +275,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -148,6 +296,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -198,7 +352,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,6 +367,22 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -292,10 +462,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S66"/>
+  <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M67" activeCellId="0" sqref="M67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G77" activeCellId="0" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4123,6 +4293,478 @@
         <v>24581</v>
       </c>
     </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="n">
+        <v>43958</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>327</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>459</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>923</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <v>828</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <v>17979</v>
+      </c>
+      <c r="J67" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="K67" s="0" t="n">
+        <v>425</v>
+      </c>
+      <c r="L67" s="0" t="n">
+        <v>794</v>
+      </c>
+      <c r="M67" s="0" t="n">
+        <v>842</v>
+      </c>
+      <c r="N67" s="0" t="n">
+        <v>1403</v>
+      </c>
+      <c r="O67" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="P67" s="0" t="n">
+        <v>548</v>
+      </c>
+      <c r="Q67" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R67" s="0" t="n">
+        <v>867</v>
+      </c>
+      <c r="S67" s="0" t="n">
+        <v>25972</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="n">
+        <v>43959</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>337</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>485</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>947</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <v>878</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>18957</v>
+      </c>
+      <c r="J68" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="K68" s="0" t="n">
+        <v>432</v>
+      </c>
+      <c r="L68" s="0" t="n">
+        <v>801</v>
+      </c>
+      <c r="M68" s="0" t="n">
+        <v>882</v>
+      </c>
+      <c r="N68" s="0" t="n">
+        <v>1418</v>
+      </c>
+      <c r="O68" s="0" t="n">
+        <v>206</v>
+      </c>
+      <c r="P68" s="0" t="n">
+        <v>559</v>
+      </c>
+      <c r="Q68" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R68" s="0" t="n">
+        <v>881</v>
+      </c>
+      <c r="S68" s="0" t="n">
+        <v>27219</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="n">
+        <v>43960</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>340</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>520</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>978</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>933</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>20353</v>
+      </c>
+      <c r="J69" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="K69" s="0" t="n">
+        <v>441</v>
+      </c>
+      <c r="L69" s="0" t="n">
+        <v>812</v>
+      </c>
+      <c r="M69" s="0" t="n">
+        <v>899</v>
+      </c>
+      <c r="N69" s="0" t="n">
+        <v>1454</v>
+      </c>
+      <c r="O69" s="0" t="n">
+        <v>206</v>
+      </c>
+      <c r="P69" s="0" t="n">
+        <v>575</v>
+      </c>
+      <c r="Q69" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R69" s="0" t="n">
+        <v>893</v>
+      </c>
+      <c r="S69" s="0" t="n">
+        <v>28866</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="n">
+        <v>43961</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>351</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>547</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>1014</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <v>970</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>21317</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="K70" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <v>814</v>
+      </c>
+      <c r="M70" s="0" t="n">
+        <v>932</v>
+      </c>
+      <c r="N70" s="0" t="n">
+        <v>1466</v>
+      </c>
+      <c r="O70" s="0" t="n">
+        <v>208</v>
+      </c>
+      <c r="P70" s="0" t="n">
+        <v>592</v>
+      </c>
+      <c r="Q70" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R70" s="0" t="n">
+        <v>901</v>
+      </c>
+      <c r="S70" s="0" t="n">
+        <v>30063</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="n">
+        <v>43962</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>351</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>578</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>1109</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <v>1029</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>22709</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>224</v>
+      </c>
+      <c r="K71" s="0" t="n">
+        <v>466</v>
+      </c>
+      <c r="L71" s="0" t="n">
+        <v>826</v>
+      </c>
+      <c r="M71" s="0" t="n">
+        <v>942</v>
+      </c>
+      <c r="N71" s="0" t="n">
+        <v>1482</v>
+      </c>
+      <c r="O71" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="P71" s="0" t="n">
+        <v>594</v>
+      </c>
+      <c r="Q71" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R71" s="0" t="n">
+        <v>910</v>
+      </c>
+      <c r="S71" s="0" t="n">
+        <v>31721</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="n">
+        <v>43963</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>359</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>615</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>1216</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="G72" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <v>1123</v>
+      </c>
+      <c r="I72" s="0" t="n">
+        <v>24965</v>
+      </c>
+      <c r="J72" s="0" t="n">
+        <v>248</v>
+      </c>
+      <c r="K72" s="0" t="n">
+        <v>485</v>
+      </c>
+      <c r="L72" s="0" t="n">
+        <v>839</v>
+      </c>
+      <c r="M72" s="0" t="n">
+        <v>975</v>
+      </c>
+      <c r="N72" s="0" t="n">
+        <v>1495</v>
+      </c>
+      <c r="O72" s="0" t="n">
+        <v>212</v>
+      </c>
+      <c r="P72" s="0" t="n">
+        <v>628</v>
+      </c>
+      <c r="Q72" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R72" s="0" t="n">
+        <v>921</v>
+      </c>
+      <c r="S72" s="0" t="n">
+        <v>34381</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="n">
+        <v>43964</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>363</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>682</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>1277</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>1213</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <v>27216</v>
+      </c>
+      <c r="J73" s="0" t="n">
+        <v>295</v>
+      </c>
+      <c r="K73" s="0" t="n">
+        <v>519</v>
+      </c>
+      <c r="L73" s="0" t="n">
+        <v>849</v>
+      </c>
+      <c r="M73" s="0" t="n">
+        <v>995</v>
+      </c>
+      <c r="N73" s="0" t="n">
+        <v>1536</v>
+      </c>
+      <c r="O73" s="0" t="n">
+        <v>214</v>
+      </c>
+      <c r="P73" s="0" t="n">
+        <v>633</v>
+      </c>
+      <c r="Q73" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R73" s="0" t="n">
+        <v>935</v>
+      </c>
+      <c r="S73" s="0" t="n">
+        <v>37040</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="n">
+        <v>43965</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>368</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>779</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>1331</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <v>1312</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <v>29276</v>
+      </c>
+      <c r="J74" s="0" t="n">
+        <v>323</v>
+      </c>
+      <c r="K74" s="0" t="n">
+        <v>540</v>
+      </c>
+      <c r="L74" s="0" t="n">
+        <v>885</v>
+      </c>
+      <c r="M74" s="0" t="n">
+        <v>1036</v>
+      </c>
+      <c r="N74" s="0" t="n">
+        <v>1564</v>
+      </c>
+      <c r="O74" s="0" t="n">
+        <v>219</v>
+      </c>
+      <c r="P74" s="0" t="n">
+        <v>641</v>
+      </c>
+      <c r="Q74" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R74" s="0" t="n">
+        <v>937</v>
+      </c>
+      <c r="S74" s="0" t="n">
+        <v>39542</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4140,10 +4782,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S66"/>
+  <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8045,6 +8687,478 @@
       </c>
       <c r="S66" s="0" t="n">
         <v>285</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="n">
+        <v>43958</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="J67" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K67" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L67" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M67" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N67" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="O67" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P67" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R67" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S67" s="0" t="n">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="n">
+        <v>43959</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="J68" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K68" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L68" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M68" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N68" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="O68" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P68" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R68" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="S68" s="0" t="n">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="n">
+        <v>43960</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="J69" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K69" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L69" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M69" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N69" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="O69" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P69" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R69" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="S69" s="0" t="n">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="n">
+        <v>43961</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K70" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M70" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N70" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="O70" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P70" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R70" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="S70" s="0" t="n">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="n">
+        <v>43962</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K71" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L71" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="M71" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N71" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="O71" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P71" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R71" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="S71" s="0" t="n">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="n">
+        <v>43963</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="I72" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="J72" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K72" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L72" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="M72" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N72" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="O72" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P72" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R72" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="S72" s="0" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="n">
+        <v>43964</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="J73" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K73" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L73" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M73" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N73" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="O73" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P73" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R73" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="S73" s="0" t="n">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="n">
+        <v>43965</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="J74" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K74" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L74" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M74" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N74" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="O74" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P74" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R74" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="S74" s="0" t="n">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -8063,10 +9177,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S66"/>
+  <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9132,6 +10246,754 @@
         <v>190</v>
       </c>
     </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="n">
+        <v>43958</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="J67" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N67" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="O67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R67" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S67" s="0" t="n">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="n">
+        <v>43959</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="J68" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L68" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M68" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P68" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R68" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S68" s="0" t="n">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="n">
+        <v>43960</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="J69" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L69" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M69" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N69" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="O69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P69" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R69" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S69" s="0" t="n">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="n">
+        <v>43961</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K70" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M70" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="N70" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P70" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R70" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="S70" s="0" t="n">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="n">
+        <v>43962</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K71" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N71" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R71" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="S71" s="0" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="n">
+        <v>43963</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I72" s="0" t="n">
+        <v>430</v>
+      </c>
+      <c r="J72" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K72" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L72" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M72" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N72" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P72" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R72" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S72" s="0" t="n">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="n">
+        <v>43964</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <v>257</v>
+      </c>
+      <c r="J73" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="K73" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N73" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P73" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S73" s="0" t="n">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="n">
+        <v>43965</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <v>267</v>
+      </c>
+      <c r="J74" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K74" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L74" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M74" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N74" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P74" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" s="0" t="n">
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="45.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>43906</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>43911</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="58.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>43930</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>43938</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>43941</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="58.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>43942</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="73.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>43945</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>43952</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>43954</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="115.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>43955</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="92.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>43956</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="47.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>43961</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>43964</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>43965</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualizado 25 de Mayo 2020
</commit_message>
<xml_diff>
--- a/casos_chile_regiones.xlsx
+++ b/casos_chile_regiones.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="91">
   <si>
     <t xml:space="preserve">fecha</t>
   </si>
@@ -135,13 +135,34 @@
     <t xml:space="preserve">Fuente</t>
   </si>
   <si>
-    <t xml:space="preserve">Fase 4</t>
+    <t xml:space="preserve">Estamos preparados para impedir que se propague</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piñera precisó que  “hemos implementado todas las recomendaciones que nos ha hecho la OMS” y aseguró que "estamos preparados para impedir que esto se propague, y por lo tanto, que los casos sean casos aislados".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piñera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.elmostrador.cl/noticias/2020/03/03/estamos-preparados-para-impedir-que-se-propague-pinera-expone-plan-de-accion-del-gobierno-para-enfrentar-el-coronavirus/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fase 4 y cierre de fronteras</t>
   </si>
   <si>
     <t xml:space="preserve">Gobierno</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsal.cl/coronavirus-en-chile-pasa-a-fase-4-y-presidente-anuncia-cierre-de-fronteras/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chile está mucho mejor preparado que Italia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"En Italia tienen 3.500 muertos y en Chile, gracias a Dios y a las precauciones que hemos tomado, aún no hemos tenido ninguno, y por lo tanto el caso de Italia va a ser muy distinto al caso de Chile y quiero darle tranquilidad a todos mis compatriotas de que Chile está mucho mejor preparado que Italia para enfrentar esta situación”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.latercera.com/politica/noticia/pinera-y-estado-de-catastrofe-podemos-confiscar-bienes-que-son-esenciales-para-las-personas-y-ponerlos-a-disposicion-de-la-gente/HUQGNFGE3NFPRII3LDS5IAHHWM/</t>
   </si>
   <si>
     <t xml:space="preserve">¿Qué pasa si el virus se vuelve buena persona?</t>
@@ -166,9 +187,6 @@
   </si>
   <si>
     <t xml:space="preserve">“no vamos a poder volver a nuestras vidas normales como eran antes, vamos a tener que acostumbrarnos a una nueva normalidad”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piñera</t>
   </si>
   <si>
     <t xml:space="preserve">https://ellibero.cl/alerta/presidente-pinera-tendremos-que-acostumbrarnos-a-una-nueva-normalidad/</t>
@@ -204,6 +222,15 @@
     <t xml:space="preserve">https://prensa.presidencia.cl/comunicado.aspx?id=150453</t>
   </si>
   <si>
+    <t xml:space="preserve">Los países que han hecho cuarentena total han fracasado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cita textual de la entrevista con Tonka Tomicic y Amaro Gómez-Pablo (Minuto 30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=rzHLJQne8iE&amp;feature=youtu.be&amp;fbclid=IwAR0DB-n-xpDZGX83rko4Ve_tYUsnrK2JROLFLYAIfGOLIBRdyK1abGf6y0k</t>
+  </si>
+  <si>
     <t xml:space="preserve">No es el momento, de Torrealba</t>
   </si>
   <si>
@@ -223,6 +250,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.24horas.cl/coronavirus/jaime-manalich-si-no-damos-con-toda-la-energia-la-batalla-de-santiago-la-guerra-del-covid-19-se-va-a-perder-4143993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estupidez humana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este domingo, el ministro del Interior, Gonzalo Blumel, condenó la fiesta clandestina donde fueron sorprendidas 400 personas, y anunció acciones legales por parte del Ejecutivo. “Esa actividad es un reflejo patente de la estupidez humana”, afirmó el secretario de Estado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blumel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.eldesconcierto.cl/2020/05/03/gonzalo-blumel-anuncia-querella-tras-fiesta-clandestina-en-maipu-es-un-reflejo-de-la-estupidez-humana/</t>
   </si>
   <si>
     <t xml:space="preserve">Irresponsabilidad de los habitantes</t>
@@ -266,6 +305,36 @@
   <si>
     <t xml:space="preserve">https://www.elmostrador.cl/noticias/pais/2020/05/14/manalich-intensamente-preocupado-ministro-apunta-a-falta-de-confianza-reciproca-para-explicar-el-complejo-cuadro-en-la-lucha-contra-el-covid-19/</t>
   </si>
+  <si>
+    <t xml:space="preserve">Chile tampoco estaba preparado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En Cadena Nacional: “Chile tampoco estaba preparado. Tenemos que ser humildes y realistas en reconocerlo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=UR393Yk-BAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vamos a llegar a cerca del 70% de las familias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En su discurso del 18 de mayo, el mandatario habló a todo el país en un punto de prensa en La Moneda, informando que “vamos a llegar a cerca del 70% de las familias”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.eldesconcierto.cl/2020/05/22/video-el-momento-en-el-quepinera-prometio-que-canastas-iban-a-llegar-al-70-de-los-chilenos/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siempre hablamos de que esto iba dirigido al 70% del 40% más pobre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El ministro de Desarrollo Social, Sebastián Sichel, aclaró el alcance de las canastas familiares anunciadas por el Gobierno. "Siempre hablamos de que esto iba dirigido al 70% del 40% más pobre. Dos millones de caja y casi dos millones 900 mil hogares, son, más o menos, el 70% (del 40 %) de los hogares más vulnerables de Chile", señaló el ministro.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sichel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.cooperativa.cl/noticias/sociedad/salud/coronavirus/ministro-sichel-canastas-llegaran-al-70-por-ciento-de-las-familias-de/2020-05-22/090612.html</t>
+  </si>
 </sst>
 </file>
 
@@ -298,7 +367,8 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -352,7 +422,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -369,16 +439,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -462,24 +528,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S74"/>
+  <dimension ref="A1:S84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G77" activeCellId="0" sqref="G77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="4.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="4.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="4.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="4.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="3" style="0" width="6.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -4763,6 +4822,596 @@
       </c>
       <c r="S74" s="0" t="n">
         <v>39542</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="n">
+        <v>43966</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>377</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>845</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>1429</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <v>1365</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>30794</v>
+      </c>
+      <c r="J75" s="0" t="n">
+        <v>329</v>
+      </c>
+      <c r="K75" s="0" t="n">
+        <v>551</v>
+      </c>
+      <c r="L75" s="0" t="n">
+        <v>921</v>
+      </c>
+      <c r="M75" s="0" t="n">
+        <v>1074</v>
+      </c>
+      <c r="N75" s="0" t="n">
+        <v>1587</v>
+      </c>
+      <c r="O75" s="0" t="n">
+        <v>219</v>
+      </c>
+      <c r="P75" s="0" t="n">
+        <v>644</v>
+      </c>
+      <c r="Q75" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R75" s="0" t="n">
+        <v>952</v>
+      </c>
+      <c r="S75" s="0" t="n">
+        <v>41428</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="n">
+        <v>43967</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>378</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>975</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>1505</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="H76" s="0" t="n">
+        <v>1474</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <v>32684</v>
+      </c>
+      <c r="J76" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="K76" s="0" t="n">
+        <v>573</v>
+      </c>
+      <c r="L76" s="0" t="n">
+        <v>942</v>
+      </c>
+      <c r="M76" s="0" t="n">
+        <v>1099</v>
+      </c>
+      <c r="N76" s="0" t="n">
+        <v>1606</v>
+      </c>
+      <c r="O76" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="P76" s="0" t="n">
+        <v>647</v>
+      </c>
+      <c r="Q76" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R76" s="0" t="n">
+        <v>961</v>
+      </c>
+      <c r="S76" s="0" t="n">
+        <v>43781</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="n">
+        <v>43968</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>398</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>1056</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>1589</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>212</v>
+      </c>
+      <c r="H77" s="0" t="n">
+        <v>1553</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <v>34451</v>
+      </c>
+      <c r="J77" s="0" t="n">
+        <v>418</v>
+      </c>
+      <c r="K77" s="0" t="n">
+        <v>602</v>
+      </c>
+      <c r="L77" s="0" t="n">
+        <v>985</v>
+      </c>
+      <c r="M77" s="0" t="n">
+        <v>1144</v>
+      </c>
+      <c r="N77" s="0" t="n">
+        <v>1639</v>
+      </c>
+      <c r="O77" s="0" t="n">
+        <v>224</v>
+      </c>
+      <c r="P77" s="0" t="n">
+        <v>652</v>
+      </c>
+      <c r="Q77" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R77" s="0" t="n">
+        <v>971</v>
+      </c>
+      <c r="S77" s="0" t="n">
+        <v>46059</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="n">
+        <v>43969</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>422</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>1109</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>1648</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <v>1639</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <v>37591</v>
+      </c>
+      <c r="J78" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="K78" s="0" t="n">
+        <v>640</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <v>988</v>
+      </c>
+      <c r="M78" s="0" t="n">
+        <v>1172</v>
+      </c>
+      <c r="N78" s="0" t="n">
+        <v>1666</v>
+      </c>
+      <c r="O78" s="0" t="n">
+        <v>229</v>
+      </c>
+      <c r="P78" s="0" t="n">
+        <v>656</v>
+      </c>
+      <c r="Q78" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R78" s="0" t="n">
+        <v>972</v>
+      </c>
+      <c r="S78" s="0" t="n">
+        <v>49579</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="n">
+        <v>43970</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>1139</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>1731</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="H79" s="0" t="n">
+        <v>1770</v>
+      </c>
+      <c r="I79" s="0" t="n">
+        <v>41179</v>
+      </c>
+      <c r="J79" s="0" t="n">
+        <v>455</v>
+      </c>
+      <c r="K79" s="0" t="n">
+        <v>680</v>
+      </c>
+      <c r="L79" s="0" t="n">
+        <v>1011</v>
+      </c>
+      <c r="M79" s="0" t="n">
+        <v>1224</v>
+      </c>
+      <c r="N79" s="0" t="n">
+        <v>1680</v>
+      </c>
+      <c r="O79" s="0" t="n">
+        <v>247</v>
+      </c>
+      <c r="P79" s="0" t="n">
+        <v>666</v>
+      </c>
+      <c r="Q79" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R79" s="0" t="n">
+        <v>977</v>
+      </c>
+      <c r="S79" s="0" t="n">
+        <v>53617</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="n">
+        <v>43971</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>453</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>1246</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>1778</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>268</v>
+      </c>
+      <c r="H80" s="0" t="n">
+        <v>1887</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <v>44641</v>
+      </c>
+      <c r="J80" s="0" t="n">
+        <v>465</v>
+      </c>
+      <c r="K80" s="0" t="n">
+        <v>731</v>
+      </c>
+      <c r="L80" s="0" t="n">
+        <v>1020</v>
+      </c>
+      <c r="M80" s="0" t="n">
+        <v>1263</v>
+      </c>
+      <c r="N80" s="0" t="n">
+        <v>1715</v>
+      </c>
+      <c r="O80" s="0" t="n">
+        <v>258</v>
+      </c>
+      <c r="P80" s="0" t="n">
+        <v>693</v>
+      </c>
+      <c r="Q80" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R80" s="0" t="n">
+        <v>987</v>
+      </c>
+      <c r="S80" s="0" t="n">
+        <v>57581</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="n">
+        <v>43972</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>471</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>1393</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>1841</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>281</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <v>48350</v>
+      </c>
+      <c r="J81" s="0" t="n">
+        <v>492</v>
+      </c>
+      <c r="K81" s="0" t="n">
+        <v>782</v>
+      </c>
+      <c r="L81" s="0" t="n">
+        <v>1025</v>
+      </c>
+      <c r="M81" s="0" t="n">
+        <v>1311</v>
+      </c>
+      <c r="N81" s="0" t="n">
+        <v>1737</v>
+      </c>
+      <c r="O81" s="0" t="n">
+        <v>262</v>
+      </c>
+      <c r="P81" s="0" t="n">
+        <v>717</v>
+      </c>
+      <c r="Q81" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R81" s="0" t="n">
+        <v>992</v>
+      </c>
+      <c r="S81" s="0" t="n">
+        <v>61857</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="n">
+        <v>43973</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>482</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>1471</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>1897</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <v>2116</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <v>51399</v>
+      </c>
+      <c r="J82" s="0" t="n">
+        <v>518</v>
+      </c>
+      <c r="K82" s="0" t="n">
+        <v>823</v>
+      </c>
+      <c r="L82" s="0" t="n">
+        <v>1077</v>
+      </c>
+      <c r="M82" s="0" t="n">
+        <v>1354</v>
+      </c>
+      <c r="N82" s="0" t="n">
+        <v>1774</v>
+      </c>
+      <c r="O82" s="0" t="n">
+        <v>274</v>
+      </c>
+      <c r="P82" s="0" t="n">
+        <v>727</v>
+      </c>
+      <c r="Q82" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R82" s="0" t="n">
+        <v>997</v>
+      </c>
+      <c r="S82" s="0" t="n">
+        <v>65393</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="n">
+        <v>43974</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>1564</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>1947</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>323</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <v>2230</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>54544</v>
+      </c>
+      <c r="J83" s="0" t="n">
+        <v>554</v>
+      </c>
+      <c r="K83" s="0" t="n">
+        <v>892</v>
+      </c>
+      <c r="L83" s="0" t="n">
+        <v>1102</v>
+      </c>
+      <c r="M83" s="0" t="n">
+        <v>1414</v>
+      </c>
+      <c r="N83" s="0" t="n">
+        <v>1808</v>
+      </c>
+      <c r="O83" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="P83" s="0" t="n">
+        <v>736</v>
+      </c>
+      <c r="Q83" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R83" s="0" t="n">
+        <v>1010</v>
+      </c>
+      <c r="S83" s="0" t="n">
+        <v>69102</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="n">
+        <v>43975</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>513</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>1630</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>2305</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>58930</v>
+      </c>
+      <c r="J84" s="0" t="n">
+        <v>588</v>
+      </c>
+      <c r="K84" s="0" t="n">
+        <v>953</v>
+      </c>
+      <c r="L84" s="0" t="n">
+        <v>1139</v>
+      </c>
+      <c r="M84" s="0" t="n">
+        <v>1458</v>
+      </c>
+      <c r="N84" s="0" t="n">
+        <v>1857</v>
+      </c>
+      <c r="O84" s="0" t="n">
+        <v>297</v>
+      </c>
+      <c r="P84" s="0" t="n">
+        <v>763</v>
+      </c>
+      <c r="Q84" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="R84" s="0" t="n">
+        <v>1016</v>
+      </c>
+      <c r="S84" s="0" t="n">
+        <v>73997</v>
       </c>
     </row>
   </sheetData>
@@ -4782,10 +5431,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S74"/>
+  <dimension ref="A1:S84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9159,6 +9808,596 @@
       </c>
       <c r="S74" s="0" t="n">
         <v>394</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="n">
+        <v>43966</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="J75" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K75" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L75" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M75" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N75" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="O75" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P75" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R75" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="S75" s="0" t="n">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="n">
+        <v>43967</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H76" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="J76" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K76" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L76" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M76" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N76" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="O76" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P76" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R76" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="S76" s="0" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="n">
+        <v>43968</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H77" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="J77" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K77" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L77" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M77" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N77" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="O77" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P77" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R77" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="S77" s="0" t="n">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="n">
+        <v>43969</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="J78" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="K78" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M78" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N78" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="O78" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P78" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R78" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="S78" s="0" t="n">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="n">
+        <v>43970</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H79" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="I79" s="0" t="n">
+        <v>348</v>
+      </c>
+      <c r="J79" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="K79" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L79" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M79" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N79" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="O79" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P79" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R79" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="S79" s="0" t="n">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="n">
+        <v>43971</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H80" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <v>388</v>
+      </c>
+      <c r="J80" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="K80" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L80" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M80" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N80" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="O80" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P80" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R80" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="S80" s="0" t="n">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="n">
+        <v>43972</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <v>423</v>
+      </c>
+      <c r="J81" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K81" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L81" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M81" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N81" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="O81" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P81" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R81" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="S81" s="0" t="n">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="n">
+        <v>43973</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <v>455</v>
+      </c>
+      <c r="J82" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="K82" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L82" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M82" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N82" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="O82" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P82" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R82" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="S82" s="0" t="n">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="n">
+        <v>43974</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>494</v>
+      </c>
+      <c r="J83" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="K83" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L83" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M83" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N83" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="O83" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P83" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R83" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="S83" s="0" t="n">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="n">
+        <v>43975</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>529</v>
+      </c>
+      <c r="J84" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K84" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L84" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="M84" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N84" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="O84" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P84" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R84" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="S84" s="0" t="n">
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -9177,10 +10416,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S74"/>
+  <dimension ref="A1:S84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10716,6 +11955,596 @@
       </c>
       <c r="S74" s="0" t="n">
         <v>390</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="n">
+        <v>43966</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="J75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L75" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="M75" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N75" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="O75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R75" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S75" s="0" t="n">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="n">
+        <v>43967</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H76" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <v>219</v>
+      </c>
+      <c r="J76" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K76" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L76" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="M76" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N76" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S76" s="0" t="n">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="n">
+        <v>43968</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H77" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="J77" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="K77" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L77" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M77" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N77" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P77" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R77" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S77" s="0" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="n">
+        <v>43969</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="J78" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="K78" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N78" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="O78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P78" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S78" s="0" t="n">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="n">
+        <v>43970</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H79" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="I79" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="J79" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K79" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L79" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M79" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N79" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S79" s="0" t="n">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="n">
+        <v>43971</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H80" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <v>336</v>
+      </c>
+      <c r="J80" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K80" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M80" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N80" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P80" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S80" s="0" t="n">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="n">
+        <v>43972</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <v>335</v>
+      </c>
+      <c r="J81" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M81" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S81" s="0" t="n">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="n">
+        <v>43973</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <v>237</v>
+      </c>
+      <c r="J82" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K82" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L82" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="M82" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N82" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="O82" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P82" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S82" s="0" t="n">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="n">
+        <v>43974</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>286</v>
+      </c>
+      <c r="J83" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K83" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L83" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M83" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N83" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="O83" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P83" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S83" s="0" t="n">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="n">
+        <v>43975</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>386</v>
+      </c>
+      <c r="J84" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K84" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M84" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N84" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="O84" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P84" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R84" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S84" s="0" t="n">
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -10734,264 +12563,383 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="45.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
-        <v>43906</v>
-      </c>
-      <c r="B2" s="0" t="s">
+        <v>43893</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
+        <v>43906</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>43908</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
         <v>43911</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="58.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="58.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
         <v>43930</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
         <v>43938</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
         <v>43941</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="58.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="58.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
         <v>43942</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="73.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
-        <v>43945</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
-        <v>43952</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>43945</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>43945</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>43952</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
         <v>43954</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="115.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="B13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>43954</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
         <v>43955</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="92.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="B15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="92.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
         <v>43956</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="47.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="47.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
         <v>43961</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="B17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
         <v>43964</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="B18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
         <v>43965</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>67</v>
+      <c r="B19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>43968</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>43969</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>43973</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>